<commit_message>
create push files on site
</commit_message>
<xml_diff>
--- a/templates/1.xlsx
+++ b/templates/1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">Школа</t>
   </si>
@@ -70,19 +70,19 @@
     <t xml:space="preserve">гор.блюдо</t>
   </si>
   <si>
-    <t xml:space="preserve">54-4г-2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">каша гречневая рассыпчатая</t>
+    <t xml:space="preserve">54-16-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Каша Дружба</t>
   </si>
   <si>
     <t xml:space="preserve">гор.напиток</t>
   </si>
   <si>
-    <t xml:space="preserve">54-8м-2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кофейный напиток</t>
+    <t xml:space="preserve">54-6гн-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чай черный байховый с молоком и сахаром</t>
   </si>
   <si>
     <t xml:space="preserve">хлеб</t>
@@ -91,22 +91,19 @@
     <t xml:space="preserve">Хлеб в ассортименте</t>
   </si>
   <si>
-    <t xml:space="preserve">54-3соус-2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">соус красный основной</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54-2р-2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Котлеты мясная</t>
+    <t xml:space="preserve">54-1з-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сыр твердых сортов</t>
   </si>
   <si>
     <t xml:space="preserve">Завтрак 2</t>
   </si>
   <si>
     <t xml:space="preserve">фрукты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Яблоко</t>
   </si>
   <si>
     <t xml:space="preserve">Обед</t>
@@ -144,7 +141,7 @@
     <numFmt numFmtId="167" formatCode="0"/>
     <numFmt numFmtId="168" formatCode="0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +167,13 @@
       <family val="0"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -337,7 +341,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -346,7 +350,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -405,6 +409,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
@@ -745,8 +753,8 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="false" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="false" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -762,7 +770,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.42"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,22 +835,22 @@
         <v>17</v>
       </c>
       <c r="E4" s="12" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="F4" s="13" t="n">
-        <v>18.5</v>
+        <v>33.15</v>
       </c>
       <c r="G4" s="12" t="n">
-        <v>262</v>
+        <v>216.6</v>
       </c>
       <c r="H4" s="12" t="n">
-        <v>8</v>
+        <v>5.1</v>
       </c>
       <c r="I4" s="12" t="n">
-        <v>6</v>
+        <v>10.9</v>
       </c>
       <c r="J4" s="14" t="n">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,29 +858,29 @@
       <c r="B5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="18" t="n">
+      <c r="E5" s="19" t="n">
         <v>200</v>
       </c>
-      <c r="F5" s="19" t="n">
-        <v>9.25</v>
-      </c>
-      <c r="G5" s="18" t="n">
-        <v>91</v>
-      </c>
-      <c r="H5" s="18" t="n">
-        <v>4</v>
-      </c>
-      <c r="I5" s="18" t="n">
-        <v>4</v>
-      </c>
-      <c r="J5" s="20" t="n">
-        <v>11</v>
+      <c r="F5" s="20" t="n">
+        <v>6.82</v>
+      </c>
+      <c r="G5" s="19" t="n">
+        <v>52.9</v>
+      </c>
+      <c r="H5" s="19" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I5" s="19" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J5" s="21" t="n">
+        <v>8.6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,248 +888,246 @@
       <c r="B6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="17" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="18" t="n">
+      <c r="E6" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="F6" s="19" t="n">
+      <c r="F6" s="20" t="n">
         <v>2.5</v>
       </c>
-      <c r="G6" s="18" t="n">
-        <v>58</v>
-      </c>
-      <c r="H6" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="20" t="n">
-        <v>12</v>
+      <c r="G6" s="19" t="n">
+        <v>57.9</v>
+      </c>
+      <c r="H6" s="19" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="I6" s="19" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J6" s="21" t="n">
+        <v>11.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="18" t="n">
-        <v>50</v>
-      </c>
-      <c r="F7" s="19" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="H7" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="18" t="n">
-        <v>5</v>
-      </c>
-      <c r="J7" s="20" t="n">
-        <v>5</v>
+      <c r="E7" s="19" t="n">
+        <v>30</v>
+      </c>
+      <c r="F7" s="20" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="G7" s="19" t="n">
+        <v>109.1</v>
+      </c>
+      <c r="H7" s="19" t="n">
+        <v>7</v>
+      </c>
+      <c r="I7" s="19" t="n">
+        <v>9</v>
+      </c>
+      <c r="J7" s="21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="27"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="B9" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="24" t="n">
-        <v>100</v>
-      </c>
-      <c r="F8" s="25" t="n">
-        <v>32</v>
-      </c>
-      <c r="G8" s="24" t="n">
-        <v>171</v>
-      </c>
-      <c r="H8" s="24" t="n">
-        <v>19</v>
-      </c>
-      <c r="I8" s="24" t="n">
-        <v>5</v>
-      </c>
-      <c r="J8" s="26" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="14"/>
+      <c r="E9" s="12" t="n">
+        <v>150</v>
+      </c>
+      <c r="F9" s="13" t="n">
+        <v>21.75</v>
+      </c>
+      <c r="G9" s="12" t="n">
+        <v>60.6</v>
+      </c>
+      <c r="H9" s="12" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I9" s="12" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J9" s="14" t="n">
+        <v>13.5</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="20"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="26"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="27"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="33"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="34"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15"/>
       <c r="B13" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="20"/>
+        <v>30</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15"/>
       <c r="B14" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="20"/>
+        <v>31</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15"/>
       <c r="B15" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="20"/>
+        <v>32</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15"/>
       <c r="B16" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="20"/>
+        <v>33</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15"/>
       <c r="B17" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="20"/>
+        <v>34</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15"/>
       <c r="B18" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="20"/>
+        <v>35</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="38"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="26"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="27"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>

</xml_diff>